<commit_message>
Results from July 27, 2020 07:56:17 AM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-27.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-27.xlsx
@@ -1085,20 +1085,20 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C14" t="n">
-        <v>104755</v>
+        <v>107315</v>
       </c>
       <c r="D14" t="n">
-        <v>1388</v>
+        <v>1404</v>
       </c>
       <c r="E14" t="n">
-        <v>9771</v>
+        <v>9879</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
-        <v>18.4</v>
+        <v>18.27</v>
       </c>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="b">
@@ -1108,7 +1108,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>53093</v>
+        <v>54066</v>
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
@@ -1130,20 +1130,20 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C15" t="n">
-        <v>26980</v>
+        <v>27393</v>
       </c>
       <c r="D15" t="n">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E15" t="n">
-        <v>3468</v>
+        <v>3513</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
-        <v>25.18</v>
+        <v>25.12</v>
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="b">
@@ -1153,7 +1153,7 @@
         <v>1</v>
       </c>
       <c r="K15" t="n">
-        <v>13773</v>
+        <v>13983</v>
       </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
@@ -1276,21 +1276,39 @@
           <t>Maryland</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
+      <c r="B18" s="2" t="n">
+        <v>44039</v>
+      </c>
+      <c r="C18" t="n">
+        <v>84876</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3315</v>
+      </c>
+      <c r="E18" t="n">
+        <v>25440</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1357</v>
+      </c>
+      <c r="G18" t="n">
+        <v>36.16</v>
+      </c>
+      <c r="H18" t="n">
+        <v>41.08</v>
+      </c>
       <c r="I18" t="b">
         <v>0</v>
       </c>
       <c r="J18" t="b">
         <v>0</v>
       </c>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
+      <c r="K18" t="n">
+        <v>70362</v>
+      </c>
+      <c r="L18" t="n">
+        <v>3303</v>
+      </c>
       <c r="M18" t="n">
         <v>1788090</v>
       </c>
@@ -1299,7 +1317,7 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>An error occurred. ... TimeoutException('', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -1549,10 +1567,10 @@
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C24" t="n">
-        <v>1400</v>
+        <v>1402</v>
       </c>
       <c r="D24" t="n">
         <v>56</v>
@@ -1564,7 +1582,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>11.7</v>
+        <v>11.67</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -1576,7 +1594,7 @@
         <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>1359</v>
+        <v>1362</v>
       </c>
       <c r="L24" t="n">
         <v>56</v>

</xml_diff>

<commit_message>
Results from July 27, 2020 11:19:42 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-27.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-27.xlsx
@@ -524,29 +524,15 @@
           <t>Texas</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>44038</v>
-      </c>
-      <c r="C2" t="n">
-        <v>32202</v>
-      </c>
-      <c r="D2" t="n">
-        <v>787</v>
-      </c>
-      <c r="E2" t="n">
-        <v>4059</v>
-      </c>
-      <c r="F2" t="n">
-        <v>99</v>
-      </c>
-      <c r="G2" t="n">
-        <v>12.6</v>
-      </c>
-      <c r="H2" t="n">
-        <v>12.58</v>
-      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>
@@ -561,7 +547,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... KeyError("None of ['Race/Ethnicity'] are in the columns")</t>
         </is>
       </c>
     </row>
@@ -572,10 +558,10 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C3" t="n">
-        <v>36083</v>
+        <v>36438</v>
       </c>
       <c r="D3" t="n">
         <v>323</v>
@@ -623,26 +609,26 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>220266</t>
+          <t>220483</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18862</t>
+          <t>18872</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>34101</v>
+        <v>34116</v>
       </c>
       <c r="F4" t="n">
-        <v>5256</v>
+        <v>5261</v>
       </c>
       <c r="G4" t="n">
-        <v>29.92</v>
+        <v>29.91</v>
       </c>
       <c r="H4" t="n">
         <v>30.44</v>
@@ -654,10 +640,10 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>113983</v>
+        <v>114053</v>
       </c>
       <c r="L4" t="n">
-        <v>17268</v>
+        <v>17283</v>
       </c>
       <c r="M4" t="n">
         <v>2049418</v>
@@ -758,25 +744,25 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C7" t="n">
-        <v>93936</v>
+        <v>96489</v>
       </c>
       <c r="D7" t="n">
-        <v>967</v>
+        <v>978</v>
       </c>
       <c r="E7" t="n">
-        <v>18149</v>
+        <v>18408</v>
       </c>
       <c r="F7" t="n">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G7" t="n">
-        <v>19.32</v>
+        <v>19.08</v>
       </c>
       <c r="H7" t="n">
-        <v>34.75</v>
+        <v>34.46</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -805,21 +791,21 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>37973</t>
+          <t>38409</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>274</t>
+          <t>281</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>941</t>
+          <t>945</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -831,7 +817,7 @@
         <v>2.5</v>
       </c>
       <c r="H8" t="n">
-        <v>1.82</v>
+        <v>1.78</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -896,22 +882,22 @@
         <v>44039</v>
       </c>
       <c r="C10" t="n">
-        <v>38623</v>
+        <v>39447</v>
       </c>
       <c r="D10" t="n">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="E10" t="n">
-        <v>8161</v>
+        <v>8264</v>
       </c>
       <c r="F10" t="n">
         <v>106</v>
       </c>
       <c r="G10" t="n">
-        <v>24.46</v>
+        <v>24.39</v>
       </c>
       <c r="H10" t="n">
-        <v>26.3</v>
+        <v>25.98</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
@@ -920,10 +906,10 @@
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>33370</v>
+        <v>33884</v>
       </c>
       <c r="L10" t="n">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="M10" t="n">
         <v>460970</v>
@@ -944,22 +930,22 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C11" t="n">
-        <v>26984</v>
+        <v>27507</v>
       </c>
       <c r="D11" t="n">
         <v>533</v>
       </c>
       <c r="E11" t="n">
-        <v>991</v>
+        <v>1012</v>
       </c>
       <c r="F11" t="n">
         <v>20</v>
       </c>
       <c r="G11" t="n">
-        <v>4.7</v>
+        <v>4.71</v>
       </c>
       <c r="H11" t="n">
         <v>3.86</v>
@@ -971,7 +957,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>21068</v>
+        <v>21477</v>
       </c>
       <c r="L11" t="n">
         <v>518</v>
@@ -1042,20 +1028,20 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C13" t="n">
-        <v>19042</v>
+        <v>19502</v>
       </c>
       <c r="D13" t="n">
-        <v>614</v>
+        <v>619</v>
       </c>
       <c r="E13" t="n">
-        <v>341</v>
+        <v>367</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
-        <v>1.79</v>
+        <v>1.88</v>
       </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="b">
@@ -1175,25 +1161,25 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C16" t="n">
-        <v>77351</v>
+        <v>79129</v>
       </c>
       <c r="D16" t="n">
-        <v>1428</v>
+        <v>1446</v>
       </c>
       <c r="E16" t="n">
-        <v>22273</v>
+        <v>22550</v>
       </c>
       <c r="F16" t="n">
-        <v>599</v>
+        <v>608</v>
       </c>
       <c r="G16" t="n">
-        <v>43.2</v>
+        <v>43.17</v>
       </c>
       <c r="H16" t="n">
-        <v>43.66</v>
+        <v>43.68</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -1202,10 +1188,10 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>51553</v>
+        <v>52230</v>
       </c>
       <c r="L16" t="n">
-        <v>1372</v>
+        <v>1392</v>
       </c>
       <c r="M16" t="n">
         <v>1293186</v>
@@ -1226,25 +1212,25 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44037</v>
+        <v>44038</v>
       </c>
       <c r="C17" t="n">
-        <v>173995</v>
+        <v>176028</v>
       </c>
       <c r="D17" t="n">
-        <v>4360</v>
+        <v>4375</v>
       </c>
       <c r="E17" t="n">
-        <v>4687</v>
+        <v>4727</v>
       </c>
       <c r="F17" t="n">
         <v>438</v>
       </c>
       <c r="G17" t="n">
-        <v>4.64</v>
+        <v>4.61</v>
       </c>
       <c r="H17" t="n">
-        <v>10.76</v>
+        <v>10.73</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
@@ -1253,10 +1239,10 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>101022</v>
+        <v>102449</v>
       </c>
       <c r="L17" t="n">
-        <v>4069</v>
+        <v>4083</v>
       </c>
       <c r="M17" t="n">
         <v>823987</v>
@@ -1328,22 +1314,22 @@
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>44037</v>
+        <v>44038</v>
       </c>
       <c r="C19" t="n">
-        <v>52304</v>
+        <v>52957</v>
       </c>
       <c r="D19" t="n">
-        <v>1495</v>
+        <v>1501</v>
       </c>
       <c r="E19" t="n">
-        <v>22670</v>
+        <v>23006</v>
       </c>
       <c r="F19" t="n">
-        <v>748</v>
+        <v>751</v>
       </c>
       <c r="G19" t="n">
-        <v>43.34</v>
+        <v>43.44</v>
       </c>
       <c r="H19" t="n">
         <v>50.03</v>
@@ -1375,16 +1361,16 @@
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C20" t="n">
-        <v>162014</v>
+        <v>163827</v>
       </c>
       <c r="D20" t="n">
-        <v>3305</v>
+        <v>3304</v>
       </c>
       <c r="E20" t="n">
-        <v>3457</v>
+        <v>3484</v>
       </c>
       <c r="F20" t="n">
         <v>97</v>
@@ -1402,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>80134</v>
+        <v>80787</v>
       </c>
       <c r="L20" t="n">
         <v>2738</v>
@@ -1429,13 +1415,13 @@
         <v>44039</v>
       </c>
       <c r="C21" t="n">
-        <v>104401</v>
+        <v>105228</v>
       </c>
       <c r="D21" t="n">
-        <v>7118</v>
+        <v>7122</v>
       </c>
       <c r="E21" t="n">
-        <v>14631</v>
+        <v>14751</v>
       </c>
       <c r="F21" t="n">
         <v>1484</v>
@@ -1453,7 +1439,7 @@
         <v>1</v>
       </c>
       <c r="K21" t="n">
-        <v>49149</v>
+        <v>49557</v>
       </c>
       <c r="L21" t="n">
         <v>6992</v>
@@ -1477,25 +1463,25 @@
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C22" t="n">
-        <v>418844</v>
+        <v>427698</v>
       </c>
       <c r="D22" t="n">
-        <v>5854</v>
+        <v>5931</v>
       </c>
       <c r="E22" t="n">
-        <v>49983</v>
+        <v>50990</v>
       </c>
       <c r="F22" t="n">
-        <v>1134</v>
+        <v>1141</v>
       </c>
       <c r="G22" t="n">
-        <v>11.93</v>
+        <v>11.92</v>
       </c>
       <c r="H22" t="n">
-        <v>19.37</v>
+        <v>19.24</v>
       </c>
       <c r="I22" t="b">
         <v>1</v>
@@ -1524,20 +1510,20 @@
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C23" t="n">
-        <v>3342</v>
+        <v>3381</v>
       </c>
       <c r="D23" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E23" t="n">
         <v>20</v>
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="b">
@@ -1618,25 +1604,25 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>44035</v>
+        <v>44038</v>
       </c>
       <c r="C25" t="n">
-        <v>46806</v>
+        <v>46994</v>
       </c>
       <c r="D25" t="n">
-        <v>3531</v>
+        <v>3536</v>
       </c>
       <c r="E25" t="n">
-        <v>6376</v>
+        <v>6436</v>
       </c>
       <c r="F25" t="n">
         <v>653</v>
       </c>
       <c r="G25" t="n">
-        <v>13.62</v>
+        <v>13.7</v>
       </c>
       <c r="H25" t="n">
-        <v>18.49</v>
+        <v>18.47</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -1665,25 +1651,25 @@
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>44036</v>
+        <v>44039</v>
       </c>
       <c r="C26" t="n">
-        <v>25109</v>
+        <v>26172</v>
       </c>
       <c r="D26" t="n">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="E26" t="n">
-        <v>1844</v>
+        <v>1931</v>
       </c>
       <c r="F26" t="n">
         <v>63</v>
       </c>
       <c r="G26" t="n">
-        <v>8.949999999999999</v>
+        <v>8.98</v>
       </c>
       <c r="H26" t="n">
-        <v>19.87</v>
+        <v>19.38</v>
       </c>
       <c r="I26" t="b">
         <v>0</v>
@@ -1692,10 +1678,10 @@
         <v>1</v>
       </c>
       <c r="K26" t="n">
-        <v>20609</v>
+        <v>21495</v>
       </c>
       <c r="L26" t="n">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="M26" t="n">
         <v>169801</v>
@@ -1716,25 +1702,25 @@
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C27" t="n">
-        <v>44336</v>
+        <v>44565</v>
       </c>
       <c r="D27" t="n">
-        <v>1794</v>
+        <v>1799</v>
       </c>
       <c r="E27" t="n">
-        <v>2088</v>
+        <v>2108</v>
       </c>
       <c r="F27" t="n">
         <v>119</v>
       </c>
       <c r="G27" t="n">
-        <v>6.08</v>
+        <v>6.09</v>
       </c>
       <c r="H27" t="n">
-        <v>6.87</v>
+        <v>6.85</v>
       </c>
       <c r="I27" t="b">
         <v>0</v>
@@ -1743,10 +1729,10 @@
         <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>34320</v>
+        <v>34627</v>
       </c>
       <c r="L27" t="n">
-        <v>1732</v>
+        <v>1737</v>
       </c>
       <c r="M27" t="n">
         <v>227938</v>
@@ -1767,22 +1753,22 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C28" t="n">
-        <v>24618</v>
+        <v>24899</v>
       </c>
       <c r="D28" t="n">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E28" t="n">
-        <v>1493</v>
+        <v>1511</v>
       </c>
       <c r="F28" t="n">
         <v>24</v>
       </c>
       <c r="G28" t="n">
-        <v>7.79</v>
+        <v>7.84</v>
       </c>
       <c r="H28" t="n">
         <v>7.92</v>
@@ -1794,7 +1780,7 @@
         <v>1</v>
       </c>
       <c r="K28" t="n">
-        <v>19165</v>
+        <v>19282</v>
       </c>
       <c r="L28" t="n">
         <v>303</v>
@@ -1818,25 +1804,25 @@
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C29" t="n">
-        <v>77930</v>
+        <v>78419</v>
       </c>
       <c r="D29" t="n">
-        <v>6071</v>
+        <v>6075</v>
       </c>
       <c r="E29" t="n">
-        <v>21877</v>
+        <v>21927</v>
       </c>
       <c r="F29" t="n">
-        <v>2420</v>
+        <v>2422</v>
       </c>
       <c r="G29" t="n">
-        <v>28.07</v>
+        <v>27.96</v>
       </c>
       <c r="H29" t="n">
-        <v>39.86</v>
+        <v>39.87</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
@@ -1868,10 +1854,10 @@
         <v>44034</v>
       </c>
       <c r="C30" t="n">
-        <v>107574</v>
+        <v>109917</v>
       </c>
       <c r="D30" t="n">
-        <v>3651</v>
+        <v>3674</v>
       </c>
       <c r="E30" t="n">
         <v>36693</v>
@@ -1916,25 +1902,25 @@
         </is>
       </c>
       <c r="B31" s="3" t="n">
-        <v>44037</v>
+        <v>44038</v>
       </c>
       <c r="C31" t="n">
-        <v>453659</v>
+        <v>460550</v>
       </c>
       <c r="D31" t="n">
-        <v>8416</v>
+        <v>8445</v>
       </c>
       <c r="E31" t="n">
-        <v>12503</v>
+        <v>12741</v>
       </c>
       <c r="F31" t="n">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="G31" t="n">
-        <v>4.3</v>
+        <v>4.32</v>
       </c>
       <c r="H31" t="n">
-        <v>8.5</v>
+        <v>8.51</v>
       </c>
       <c r="I31" t="b">
         <v>0</v>
@@ -1943,10 +1929,10 @@
         <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>290599</v>
+        <v>295103</v>
       </c>
       <c r="L31" t="n">
-        <v>8197</v>
+        <v>8238</v>
       </c>
       <c r="M31" t="n">
         <v>2267875</v>
@@ -1967,25 +1953,25 @@
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C32" t="n">
-        <v>62372</v>
+        <v>62907</v>
       </c>
       <c r="D32" t="n">
-        <v>2706</v>
+        <v>2709</v>
       </c>
       <c r="E32" t="n">
-        <v>6966</v>
+        <v>7242</v>
       </c>
       <c r="F32" t="n">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="G32" t="n">
-        <v>11.17</v>
+        <v>11.51</v>
       </c>
       <c r="H32" t="n">
-        <v>14.12</v>
+        <v>14.14</v>
       </c>
       <c r="I32" t="b">
         <v>1</v>
@@ -2014,22 +2000,22 @@
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C33" t="n">
-        <v>1597</v>
+        <v>1638</v>
       </c>
       <c r="D33" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E33" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>4.77</v>
+        <v>4.78</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -2041,10 +2027,10 @@
         <v>1</v>
       </c>
       <c r="K33" t="n">
-        <v>1468</v>
+        <v>1506</v>
       </c>
       <c r="L33" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M33" t="n">
         <v>24129</v>
@@ -2065,25 +2051,25 @@
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C34" t="n">
-        <v>48827</v>
+        <v>49417</v>
       </c>
       <c r="D34" t="n">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="E34" t="n">
-        <v>7558</v>
+        <v>7632</v>
       </c>
       <c r="F34" t="n">
         <v>201</v>
       </c>
       <c r="G34" t="n">
-        <v>17.16</v>
+        <v>17.12</v>
       </c>
       <c r="H34" t="n">
-        <v>22.95</v>
+        <v>22.92</v>
       </c>
       <c r="I34" t="b">
         <v>0</v>
@@ -2092,10 +2078,10 @@
         <v>1</v>
       </c>
       <c r="K34" t="n">
-        <v>44055</v>
+        <v>44574</v>
       </c>
       <c r="L34" t="n">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="M34" t="n">
         <v>368744</v>
@@ -2116,25 +2102,25 @@
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C35" t="n">
-        <v>167953</v>
+        <v>170843</v>
       </c>
       <c r="D35" t="n">
-        <v>3498</v>
+        <v>3509</v>
       </c>
       <c r="E35" t="n">
-        <v>43532</v>
+        <v>43914</v>
       </c>
       <c r="F35" t="n">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="G35" t="n">
-        <v>25.92</v>
+        <v>25.7</v>
       </c>
       <c r="H35" t="n">
-        <v>45.65</v>
+        <v>45.54</v>
       </c>
       <c r="I35" t="b">
         <v>1</v>
@@ -2163,16 +2149,16 @@
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C36" t="n">
-        <v>52635</v>
+        <v>53321</v>
       </c>
       <c r="D36" t="n">
-        <v>1501</v>
+        <v>1518</v>
       </c>
       <c r="E36" t="n">
-        <v>1903</v>
+        <v>1930</v>
       </c>
       <c r="F36" t="n">
         <v>49</v>
@@ -2181,7 +2167,7 @@
         <v>5.44</v>
       </c>
       <c r="H36" t="n">
-        <v>3.35</v>
+        <v>3.31</v>
       </c>
       <c r="I36" t="b">
         <v>0</v>
@@ -2190,10 +2176,10 @@
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>34993</v>
+        <v>35454</v>
       </c>
       <c r="L36" t="n">
-        <v>1464</v>
+        <v>1479</v>
       </c>
       <c r="M36" t="n">
         <v>269854</v>
@@ -2214,10 +2200,10 @@
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C37" t="n">
-        <v>6436</v>
+        <v>6441</v>
       </c>
       <c r="D37" t="n">
         <v>409</v>
@@ -2229,7 +2215,7 @@
         <v>9</v>
       </c>
       <c r="G37" t="n">
-        <v>6.01</v>
+        <v>5.99</v>
       </c>
       <c r="H37" t="n">
         <v>2.22</v>
@@ -2241,7 +2227,7 @@
         <v>0</v>
       </c>
       <c r="K37" t="n">
-        <v>5577</v>
+        <v>5595</v>
       </c>
       <c r="L37" t="n">
         <v>406</v>
@@ -2334,7 +2320,7 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>An error occurred. ... HTTPError('504 Server Error: Gateway Time-out for url: https://myhealthycommunity.dhss.delaware.gov/locations/state/')</t>
+          <t>An error occurred. ... AttributeError("'numpy.float64' object has no attribute 'split'")</t>
         </is>
       </c>
     </row>
@@ -2390,25 +2376,25 @@
         </is>
       </c>
       <c r="B41" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C41" t="n">
-        <v>42485</v>
+        <v>42700</v>
       </c>
       <c r="D41" t="n">
-        <v>829</v>
+        <v>836</v>
       </c>
       <c r="E41" t="n">
-        <v>3371</v>
+        <v>3391</v>
       </c>
       <c r="F41" t="n">
         <v>38</v>
       </c>
       <c r="G41" t="n">
-        <v>7.93</v>
+        <v>7.94</v>
       </c>
       <c r="H41" t="n">
-        <v>4.58</v>
+        <v>4.55</v>
       </c>
       <c r="I41" t="b">
         <v>1</v>
@@ -2437,25 +2423,25 @@
         </is>
       </c>
       <c r="B42" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C42" t="n">
-        <v>112713</v>
+        <v>114338</v>
       </c>
       <c r="D42" t="n">
-        <v>1785</v>
+        <v>1790</v>
       </c>
       <c r="E42" t="n">
-        <v>19045</v>
+        <v>19338</v>
       </c>
       <c r="F42" t="n">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="G42" t="n">
-        <v>23.99</v>
+        <v>24.01</v>
       </c>
       <c r="H42" t="n">
-        <v>32.39</v>
+        <v>32.43</v>
       </c>
       <c r="I42" t="b">
         <v>0</v>
@@ -2464,10 +2450,10 @@
         <v>1</v>
       </c>
       <c r="K42" t="n">
-        <v>79387</v>
+        <v>80533</v>
       </c>
       <c r="L42" t="n">
-        <v>1723</v>
+        <v>1727</v>
       </c>
       <c r="M42" t="n">
         <v>2179622</v>
@@ -2488,25 +2474,25 @@
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C43" t="n">
-        <v>171424</v>
+        <v>172655</v>
       </c>
       <c r="D43" t="n">
-        <v>7398</v>
+        <v>7416</v>
       </c>
       <c r="E43" t="n">
-        <v>28568</v>
+        <v>28718</v>
       </c>
       <c r="F43" t="n">
-        <v>2033</v>
+        <v>2036</v>
       </c>
       <c r="G43" t="n">
-        <v>16.67</v>
+        <v>16.63</v>
       </c>
       <c r="H43" t="n">
-        <v>27.48</v>
+        <v>27.45</v>
       </c>
       <c r="I43" t="b">
         <v>1</v>
@@ -2535,25 +2521,25 @@
         </is>
       </c>
       <c r="B44" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C44" t="n">
-        <v>18177</v>
+        <v>18694</v>
       </c>
       <c r="D44" t="n">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="E44" t="n">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F44" t="n">
         <v>3</v>
       </c>
       <c r="G44" t="n">
-        <v>1.23</v>
+        <v>1.2</v>
       </c>
       <c r="H44" t="n">
-        <v>2.13</v>
+        <v>2</v>
       </c>
       <c r="I44" t="b">
         <v>0</v>
@@ -2581,21 +2567,39 @@
           <t>Ohio</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
+      <c r="B45" s="2" t="n">
+        <v>44039</v>
+      </c>
+      <c r="C45" t="n">
+        <v>85177</v>
+      </c>
+      <c r="D45" t="n">
+        <v>3344</v>
+      </c>
+      <c r="E45" t="n">
+        <v>21687</v>
+      </c>
+      <c r="F45" t="n">
+        <v>649</v>
+      </c>
+      <c r="G45" t="n">
+        <v>29.48</v>
+      </c>
+      <c r="H45" t="n">
+        <v>19.75</v>
+      </c>
       <c r="I45" t="b">
         <v>0</v>
       </c>
       <c r="J45" t="b">
-        <v>0</v>
-      </c>
-      <c r="K45" t="inlineStr"/>
-      <c r="L45" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K45" t="n">
+        <v>73562</v>
+      </c>
+      <c r="L45" t="n">
+        <v>3286</v>
+      </c>
       <c r="M45" t="n">
         <v>1438271</v>
       </c>
@@ -2604,7 +2608,7 @@
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>An error occurred. ... JSONDecodeError('Expecting value: line 1 column 1 (char 0)')</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -2615,25 +2619,25 @@
         </is>
       </c>
       <c r="B46" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C46" t="n">
-        <v>51153</v>
+        <v>51803</v>
       </c>
       <c r="D46" t="n">
-        <v>1574</v>
+        <v>1576</v>
       </c>
       <c r="E46" t="n">
-        <v>10500</v>
+        <v>10638</v>
       </c>
       <c r="F46" t="n">
         <v>149</v>
       </c>
       <c r="G46" t="n">
-        <v>20.53</v>
+        <v>20.54</v>
       </c>
       <c r="H46" t="n">
-        <v>9.470000000000001</v>
+        <v>9.449999999999999</v>
       </c>
       <c r="I46" t="b">
         <v>1</v>
@@ -2662,16 +2666,16 @@
         </is>
       </c>
       <c r="B47" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C47" t="n">
-        <v>115637</v>
+        <v>115926</v>
       </c>
       <c r="D47" t="n">
-        <v>8529</v>
+        <v>8536</v>
       </c>
       <c r="E47" t="n">
-        <v>10824</v>
+        <v>10845</v>
       </c>
       <c r="F47" t="n">
         <v>699</v>
@@ -2680,7 +2684,7 @@
         <v>9.359999999999999</v>
       </c>
       <c r="H47" t="n">
-        <v>8.199999999999999</v>
+        <v>8.19</v>
       </c>
       <c r="I47" t="b">
         <v>1</v>
@@ -2709,25 +2713,25 @@
         </is>
       </c>
       <c r="B48" s="2" t="n">
-        <v>44036</v>
+        <v>44039</v>
       </c>
       <c r="C48" t="n">
-        <v>17655</v>
+        <v>18261</v>
       </c>
       <c r="D48" t="n">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="E48" t="n">
-        <v>4964</v>
+        <v>5149</v>
       </c>
       <c r="F48" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G48" t="n">
-        <v>30.36</v>
+        <v>30.44</v>
       </c>
       <c r="H48" t="n">
-        <v>39.3</v>
+        <v>39.05</v>
       </c>
       <c r="I48" t="b">
         <v>0</v>
@@ -2736,10 +2740,10 @@
         <v>0</v>
       </c>
       <c r="K48" t="n">
-        <v>16352</v>
+        <v>16918</v>
       </c>
       <c r="L48" t="n">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="M48" t="n">
         <v>252321</v>
@@ -2760,25 +2764,25 @@
         </is>
       </c>
       <c r="B49" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C49" t="n">
-        <v>41925</v>
+        <v>43045</v>
       </c>
       <c r="D49" t="n">
-        <v>1197</v>
+        <v>1201</v>
       </c>
       <c r="E49" t="n">
-        <v>9113</v>
+        <v>9264</v>
       </c>
       <c r="F49" t="n">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="G49" t="n">
-        <v>28.55</v>
+        <v>28.41</v>
       </c>
       <c r="H49" t="n">
-        <v>34.24</v>
+        <v>34.17</v>
       </c>
       <c r="I49" t="b">
         <v>0</v>
@@ -2787,10 +2791,10 @@
         <v>1</v>
       </c>
       <c r="K49" t="n">
-        <v>31924</v>
+        <v>32609</v>
       </c>
       <c r="L49" t="n">
-        <v>1142</v>
+        <v>1156</v>
       </c>
       <c r="M49" t="n">
         <v>704896</v>
@@ -2811,21 +2815,21 @@
         </is>
       </c>
       <c r="B50" s="2" t="n">
-        <v>44037</v>
+        <v>44038</v>
       </c>
       <c r="C50" t="n">
-        <v>411736</v>
+        <v>412344</v>
       </c>
       <c r="D50" t="n">
-        <v>25106</v>
+        <v>25117</v>
       </c>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="n">
-        <v>6349</v>
+        <v>6354</v>
       </c>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="n">
-        <v>26.9</v>
+        <v>26.91</v>
       </c>
       <c r="I50" t="b">
         <v>0</v>
@@ -2835,7 +2839,7 @@
       </c>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="n">
-        <v>23598</v>
+        <v>23614</v>
       </c>
       <c r="M50" t="inlineStr"/>
       <c r="N50" t="inlineStr"/>

</xml_diff>